<commit_message>
Converter date format changed to DD.MM.YYYY; Auto uncheck insurance; Client list form resize
</commit_message>
<xml_diff>
--- a/converter/input.xlsx
+++ b/converter/input.xlsx
@@ -30,7 +30,7 @@
     <author>Philipp Grigoryev</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,10 +39,11 @@
             <i val="false"/>
             <strike val="false"/>
             <color rgb="FF 0 0 0"/>
-            <sz val="8"/>
-            <u val="none"/>
-          </rPr>
-          <t xml:space="preserve">255 символов</t>
+            <sz val="9"/>
+            <u val="none"/>
+          </rPr>
+          <t xml:space="preserve">Philipp Grigoryev:
+М или Ж</t>
         </r>
         <r>
           <rPr>
@@ -87,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -96,11 +97,10 @@
             <i val="false"/>
             <strike val="false"/>
             <color rgb="FF 0 0 0"/>
-            <sz val="9"/>
-            <u val="none"/>
-          </rPr>
-          <t xml:space="preserve">Philipp Grigoryev:
-М или Ж</t>
+            <sz val="8"/>
+            <u val="none"/>
+          </rPr>
+          <t xml:space="preserve">255 символов</t>
         </r>
         <r>
           <rPr>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5" count="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4" count="4">
   <si>
     <t>М</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>М</t>
-  </si>
-  <si>
-    <t>1970-01-01</t>
   </si>
 </sst>
 </file>
@@ -168,10 +165,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="0">
+    <border diagonalUp="0" diagonalDown="0">
       <right style="none">
         <color rgb="FFC7C7C7"/>
       </right>
+      <top style="none">
+        <color rgb="FFC7C7C7"/>
+      </top>
     </border>
     <border diagonalUp="0" diagonalDown="0">
       <left style="none">
@@ -218,7 +218,7 @@
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0" tabSelected="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -285,13 +285,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>1111111111</v>
+        <v>4507120315</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
       </c>
       <c r="H2" t="str">
-        <v>1960-01-01</v>
+        <v>30.02.1960</v>
       </c>
       <c r="I2" t="str">
         <v>Альметьевск</v>
@@ -314,13 +314,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>2222222222</v>
+        <v>4004047028</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
-        <v>4</v>
+      <c r="H3" t="str">
+        <v>01.01.1970</v>
       </c>
       <c r="I3" t="str">
         <v>Урюпинск</v>
@@ -346,13 +346,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>3333333333</v>
+        <v>4507887863</v>
       </c>
       <c r="G4" t="s">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
-        <v>4</v>
+      <c r="H4" t="str">
+        <v>02.02.1970</v>
       </c>
       <c r="I4" t="str">
         <v>Москва</v>
@@ -377,14 +377,14 @@
       <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" t="str">
-        <v>4444444444</v>
+      <c r="F5">
+        <v>4507887843</v>
       </c>
       <c r="G5" t="s">
         <v>2</v>
       </c>
       <c r="H5" t="str">
-        <v>1950-01-01</v>
+        <v>03.03.1950</v>
       </c>
       <c r="I5" t="str">
         <v>Полтава</v>

</xml_diff>